<commit_message>
lfo rates sync off
</commit_message>
<xml_diff>
--- a/edisyn/synth/asmhydrasynth/info/nrpn.xlsx
+++ b/edisyn/synth/asmhydrasynth/info/nrpn.xlsx
@@ -2191,7 +2191,8 @@
     <t>[0,8192] seemingly only output in increments of 8, and displayed as [0.02 Hz ...150.00 Hz]. To display: if 8192, display 150.00Hz.  Else divide by 6.4 (cutting into 1280 even pieces).  Now we need to map to an exponential function to get the Hz value.  It seems the following function is a pretty close fit:  
 2^(1 + 0.012571 *  v) / 100   -I would then display as x.xx, perhaps rounded down.  Would be nice to know what their exact function is.</t>
+I would then display as x.xx, perhaps rounded down.  Would be nice to know what their exact function is.
+Edit: Benny Rönnhager manually went through the entire list, and reports the following values for all elements [0...8192] in multiples of 8, that is, [0...1024]:   LFO_RATES_SYNC_OFF    However I have not verified it yet.</t>
   </si>
   <si>
     <t>lfo1ratesyncon</t>
@@ -10341,7 +10342,7 @@
     <col min="1" max="1" width="22.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.4375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.72656" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="69.8047" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10885,7 +10886,7 @@
       </c>
       <c r="D50" s="9"/>
     </row>
-    <row r="51" ht="248.35" customHeight="1">
+    <row r="51" ht="260.35" customHeight="1">
       <c r="A51" t="s" s="6">
         <v>100</v>
       </c>
@@ -11741,7 +11742,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="127" ht="56.35" customHeight="1">
+    <row r="127" ht="68.35" customHeight="1">
       <c r="A127" t="s" s="6">
         <v>292</v>
       </c>
@@ -12241,7 +12242,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="167" ht="32.35" customHeight="1">
+    <row r="167" ht="44.35" customHeight="1">
       <c r="A167" t="s" s="6">
         <v>407</v>
       </c>
@@ -12449,7 +12450,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="184" ht="56.35" customHeight="1">
+    <row r="184" ht="68.35" customHeight="1">
       <c r="A184" t="s" s="6">
         <v>452</v>
       </c>
@@ -12533,7 +12534,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="191" ht="116.35" customHeight="1">
+    <row r="191" ht="164.35" customHeight="1">
       <c r="A191" t="s" s="6">
         <v>467</v>
       </c>
@@ -12559,7 +12560,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="193" ht="104.35" customHeight="1">
+    <row r="193" ht="116.35" customHeight="1">
       <c r="A193" t="s" s="6">
         <v>474</v>
       </c>
@@ -16337,7 +16338,7 @@
       </c>
       <c r="D568" s="9"/>
     </row>
-    <row r="569" ht="188.35" customHeight="1">
+    <row r="569" ht="200.35" customHeight="1">
       <c r="A569" t="s" s="6">
         <v>1191</v>
       </c>
@@ -16375,7 +16376,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="572" ht="200.35" customHeight="1">
+    <row r="572" ht="212.35" customHeight="1">
       <c r="A572" t="s" s="6">
         <v>1201</v>
       </c>
@@ -16403,7 +16404,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="574" ht="200.35" customHeight="1">
+    <row r="574" ht="212.35" customHeight="1">
       <c r="A574" t="s" s="6">
         <v>1208</v>
       </c>
@@ -17687,7 +17688,7 @@
       </c>
       <c r="D691" s="9"/>
     </row>
-    <row r="692" ht="44.35" customHeight="1">
+    <row r="692" ht="56.35" customHeight="1">
       <c r="A692" t="s" s="6">
         <v>1448</v>
       </c>
@@ -22151,7 +22152,7 @@
         <v>2203</v>
       </c>
     </row>
-    <row r="1123" ht="104.35" customHeight="1">
+    <row r="1123" ht="116.35" customHeight="1">
       <c r="A1123" t="s" s="26">
         <v>2204</v>
       </c>
@@ -22227,7 +22228,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="1129" ht="164.35" customHeight="1">
+    <row r="1129" ht="248.35" customHeight="1">
       <c r="A1129" t="s" s="26">
         <v>2212</v>
       </c>
@@ -22779,7 +22780,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="1180" ht="44.35" customHeight="1">
+    <row r="1180" ht="56.35" customHeight="1">
       <c r="A1180" t="s" s="6">
         <v>2296</v>
       </c>
@@ -22791,7 +22792,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="1181" ht="20.35" customHeight="1">
+    <row r="1181" ht="32.35" customHeight="1">
       <c r="A1181" t="s" s="6">
         <v>2299</v>
       </c>
@@ -22803,7 +22804,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1182" ht="20.35" customHeight="1">
+    <row r="1182" ht="32.35" customHeight="1">
       <c r="A1182" t="s" s="6">
         <v>2302</v>
       </c>
@@ -22815,7 +22816,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1183" ht="20.35" customHeight="1">
+    <row r="1183" ht="32.35" customHeight="1">
       <c r="A1183" t="s" s="6">
         <v>2304</v>
       </c>
@@ -22827,7 +22828,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1184" ht="20.35" customHeight="1">
+    <row r="1184" ht="32.35" customHeight="1">
       <c r="A1184" t="s" s="6">
         <v>2306</v>
       </c>
@@ -22839,7 +22840,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1185" ht="44.35" customHeight="1">
+    <row r="1185" ht="56.35" customHeight="1">
       <c r="A1185" t="s" s="6">
         <v>2308</v>
       </c>
@@ -22851,7 +22852,7 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="1186" ht="20.35" customHeight="1">
+    <row r="1186" ht="32.35" customHeight="1">
       <c r="A1186" t="s" s="6">
         <v>2310</v>
       </c>
@@ -22863,7 +22864,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1187" ht="20.35" customHeight="1">
+    <row r="1187" ht="32.35" customHeight="1">
       <c r="A1187" t="s" s="6">
         <v>2312</v>
       </c>
@@ -22875,7 +22876,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1188" ht="20.35" customHeight="1">
+    <row r="1188" ht="32.35" customHeight="1">
       <c r="A1188" t="s" s="6">
         <v>2314</v>
       </c>
@@ -22887,7 +22888,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="1189" ht="20.35" customHeight="1">
+    <row r="1189" ht="32.35" customHeight="1">
       <c r="A1189" t="s" s="6">
         <v>2316</v>
       </c>
@@ -24205,7 +24206,7 @@
         <v>2082</v>
       </c>
     </row>
-    <row r="1309" ht="44.35" customHeight="1">
+    <row r="1309" ht="56.35" customHeight="1">
       <c r="A1309" t="s" s="6">
         <v>2341</v>
       </c>

</xml_diff>